<commit_message>
zip file returned and download
</commit_message>
<xml_diff>
--- a/Backend/BCE7518_COMPUTER_VISION.xlsx
+++ b/Backend/BCE7518_COMPUTER_VISION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sachi\OneDrive\Desktop\Question Paper Generator\Updated Backend Host\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe3b244c9c926f8f/Desktop/Question Paper Generator/exam-engine-frontend/Backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4FAFA4-41C0-497B-BE9C-2082A199B40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Question Paper - General Inform" sheetId="1" r:id="rId1"/>
@@ -2636,7 +2636,7 @@
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -2865,8 +2865,8 @@
   </sheetPr>
   <dimension ref="A1:M301"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" zoomScale="87" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="J78" sqref="J78"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>